<commit_message>
Fixed issue - two digits missing for compensation number.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="128">
   <si>
     <t>Name</t>
   </si>
@@ -424,6 +424,18 @@
   </si>
   <si>
     <t>1128_VendorNames</t>
+  </si>
+  <si>
+    <t>1128_API_Environment</t>
+  </si>
+  <si>
+    <t>API_Environment</t>
+  </si>
+  <si>
+    <t>Robot Finished Processing</t>
+  </si>
+  <si>
+    <t>Hi, Robot successfully finished Order Finalization &amp; Claim Settlement. Regards, EC_JD Robot.</t>
   </si>
 </sst>
 </file>
@@ -780,7 +792,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +883,7 @@
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,10 +1084,16 @@
       <c r="A24" t="s">
         <v>92</v>
       </c>
+      <c r="B24" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1158,10 +1176,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="65.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,6 +1387,14 @@
         <v>123</v>
       </c>
     </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added System and Business Exception Email Notification Fixed Order Verified status not captured Fixed same store second order entry has error.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="136">
   <si>
     <t>Name</t>
   </si>
@@ -436,6 +436,41 @@
   </si>
   <si>
     <t>Hi, Robot successfully finished Order Finalization &amp; Claim Settlement. Regards, EC_JD Robot.</t>
+  </si>
+  <si>
+    <t>BusinessException_MailSubject</t>
+  </si>
+  <si>
+    <t>BusinessException_MailBody</t>
+  </si>
+  <si>
+    <t>Business Exception - OrderID:&lt;OrderID&gt;</t>
+  </si>
+  <si>
+    <t>Hi,
+Business Exception ocurred
+OrderID:&lt;OrderID&gt; 
+Business Exception Message:&lt;ExceptionMessage&gt;
+Regards,
+RPA JD Robot.</t>
+  </si>
+  <si>
+    <t>RPA System Exception - OrderID:&lt;OrderID&gt;</t>
+  </si>
+  <si>
+    <t>SystemException_MailSubject</t>
+  </si>
+  <si>
+    <t>SystemException_MailBody</t>
+  </si>
+  <si>
+    <t>Hi,
+System Exception ocurred
+OrderID:&lt;OrderID&gt; 
+System Exception Message:&lt;ExceptionMessage&gt;
+Stack Trace/Error Details:&lt;StackTrace&gt;
+Regards,
+RPA JD Robot.</t>
   </si>
 </sst>
 </file>
@@ -789,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,6 +905,38 @@
       </c>
       <c r="B8" s="2" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1178,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="65.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>